<commit_message>
fix fubar data and add new rmd file
</commit_message>
<xml_diff>
--- a/Data for bill stat class.xlsx
+++ b/Data for bill stat class.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Project_folders\Zia2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project_folders\Zia2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -116,9 +116,6 @@
     <t>mostly clear</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>Waxing Cresent</t>
   </si>
   <si>
@@ -202,22 +199,24 @@
   <si>
     <t>full moon</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="h&quot;:&quot;mm"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="h&quot;:&quot;mm&quot; &quot;AM/PM"/>
     <numFmt numFmtId="168" formatCode="#,##0.0"/>
     <numFmt numFmtId="169" formatCode="d\-mmm\-yyyy"/>
-    <numFmt numFmtId="170" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="171" formatCode="d\-mmmm"/>
-    <numFmt numFmtId="172" formatCode="d\-mmmm\-yy"/>
-    <numFmt numFmtId="173" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="170" formatCode="d\-mmmm"/>
+    <numFmt numFmtId="171" formatCode="d\-mmmm\-yy"/>
+    <numFmt numFmtId="172" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -1094,13 +1093,13 @@
     <xf numFmtId="169" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="2" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1176,10 +1175,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1192,14 +1191,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1209,7 +1208,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1550,8 +1549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="L61" workbookViewId="0">
+      <selection activeCell="L83" sqref="L83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -3828,9 +3827,7 @@
         <v>18</v>
       </c>
       <c r="O39" s="87"/>
-      <c r="P39" s="88" t="s">
-        <v>30</v>
-      </c>
+      <c r="P39" s="88"/>
       <c r="Q39" s="89"/>
       <c r="R39" s="22"/>
       <c r="S39" s="23"/>
@@ -3876,7 +3873,7 @@
         <v>0</v>
       </c>
       <c r="L40" s="97" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M40" s="96">
         <v>37</v>
@@ -3935,7 +3932,7 @@
         <v>0</v>
       </c>
       <c r="L41" s="97" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M41" s="96">
         <v>37</v>
@@ -3994,7 +3991,7 @@
         <v>0</v>
       </c>
       <c r="L42" s="97" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M42" s="96">
         <v>37</v>
@@ -4053,7 +4050,7 @@
         <v>0.6</v>
       </c>
       <c r="L43" s="97" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M43" s="87">
         <v>37</v>
@@ -4112,7 +4109,7 @@
         <v>0</v>
       </c>
       <c r="L44" s="111" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M44" s="96">
         <v>46</v>
@@ -4171,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="L45" s="97" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M45" s="96">
         <v>46</v>
@@ -4230,7 +4227,7 @@
         <v>0.6</v>
       </c>
       <c r="L46" s="97" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M46" s="87">
         <v>46</v>
@@ -4295,7 +4292,7 @@
         <v>66</v>
       </c>
       <c r="N47" s="108" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O47" s="112" t="s">
         <v>19</v>
@@ -4348,13 +4345,13 @@
         <v>3</v>
       </c>
       <c r="L48" s="97" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M48" s="96">
         <v>71.400000000000006</v>
       </c>
       <c r="N48" s="95" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O48" s="98" t="s">
         <v>19</v>
@@ -4407,13 +4404,13 @@
         <v>0.7</v>
       </c>
       <c r="L49" s="97" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M49" s="96">
         <v>71.400000000000006</v>
       </c>
       <c r="N49" s="95" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O49" s="100" t="s">
         <v>19</v>
@@ -4472,12 +4469,10 @@
         <v>99</v>
       </c>
       <c r="N50" s="129" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O50" s="129"/>
-      <c r="P50" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P50" s="132"/>
       <c r="Q50" s="89"/>
       <c r="R50" s="22"/>
       <c r="S50" s="23"/>
@@ -4523,18 +4518,16 @@
         <v>0.7</v>
       </c>
       <c r="L51" s="131" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M51" s="129">
         <v>94.7</v>
       </c>
       <c r="N51" s="129" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O51" s="129"/>
-      <c r="P51" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P51" s="132"/>
       <c r="Q51" s="89"/>
       <c r="R51" s="22"/>
       <c r="S51" s="23"/>
@@ -4580,7 +4573,7 @@
         <v>0.7</v>
       </c>
       <c r="L52" s="131" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M52" s="129">
         <v>58</v>
@@ -4589,9 +4582,7 @@
         <v>18</v>
       </c>
       <c r="O52" s="129"/>
-      <c r="P52" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P52" s="132"/>
       <c r="Q52" s="89"/>
       <c r="R52" s="22"/>
       <c r="S52" s="23"/>
@@ -4646,9 +4637,7 @@
         <v>18</v>
       </c>
       <c r="O53" s="129"/>
-      <c r="P53" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P53" s="132"/>
       <c r="Q53" s="89"/>
       <c r="R53" s="22"/>
       <c r="S53" s="23"/>
@@ -4694,7 +4683,7 @@
         <v>0</v>
       </c>
       <c r="L54" s="131" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M54" s="129">
         <v>72</v>
@@ -4703,9 +4692,7 @@
         <v>18</v>
       </c>
       <c r="O54" s="129"/>
-      <c r="P54" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P54" s="132"/>
       <c r="Q54" s="89"/>
       <c r="R54" s="22"/>
       <c r="S54" s="23"/>
@@ -4751,7 +4738,7 @@
         <v>0.5</v>
       </c>
       <c r="L55" s="131" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M55" s="129">
         <v>44.4</v>
@@ -4760,9 +4747,7 @@
         <v>18</v>
       </c>
       <c r="O55" s="129"/>
-      <c r="P55" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P55" s="132"/>
       <c r="Q55" s="89"/>
       <c r="R55" s="22"/>
       <c r="S55" s="23"/>
@@ -4808,7 +4793,7 @@
         <v>0.6</v>
       </c>
       <c r="L56" s="131" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M56" s="129">
         <v>7</v>
@@ -4817,9 +4802,7 @@
         <v>18</v>
       </c>
       <c r="O56" s="129"/>
-      <c r="P56" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P56" s="132"/>
       <c r="Q56" s="89"/>
       <c r="R56" s="22"/>
       <c r="S56" s="23"/>
@@ -4865,18 +4848,16 @@
         <v>0</v>
       </c>
       <c r="L57" s="131" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M57" s="129">
         <v>97</v>
       </c>
       <c r="N57" s="129" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O57" s="129"/>
-      <c r="P57" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P57" s="132"/>
       <c r="Q57" s="89"/>
       <c r="R57" s="22"/>
       <c r="S57" s="23"/>
@@ -4922,7 +4903,7 @@
         <v>0.5</v>
       </c>
       <c r="L58" s="131" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M58" s="129">
         <v>13.3</v>
@@ -4931,9 +4912,7 @@
         <v>18</v>
       </c>
       <c r="O58" s="129"/>
-      <c r="P58" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P58" s="132"/>
       <c r="Q58" s="89"/>
       <c r="R58" s="22"/>
       <c r="S58" s="23"/>
@@ -4979,18 +4958,16 @@
         <v>0.5</v>
       </c>
       <c r="L59" s="131" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M59" s="129">
         <v>78.599999999999994</v>
       </c>
       <c r="N59" s="129" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O59" s="129"/>
-      <c r="P59" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P59" s="132"/>
       <c r="Q59" s="89"/>
       <c r="R59" s="22"/>
       <c r="S59" s="23"/>
@@ -5036,7 +5013,7 @@
         <v>2.5</v>
       </c>
       <c r="L60" s="131" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M60" s="129">
         <v>26.3</v>
@@ -5045,9 +5022,7 @@
         <v>18</v>
       </c>
       <c r="O60" s="129"/>
-      <c r="P60" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P60" s="132"/>
       <c r="Q60" s="89"/>
       <c r="R60" s="22"/>
       <c r="S60" s="23"/>
@@ -5069,7 +5044,7 @@
         <v>60</v>
       </c>
       <c r="D61" s="136" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E61" s="137">
         <v>0.90763888888888888</v>
@@ -5093,7 +5068,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="L61" s="131" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M61" s="129">
         <v>48.9</v>
@@ -5102,9 +5077,7 @@
         <v>18</v>
       </c>
       <c r="O61" s="129"/>
-      <c r="P61" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P61" s="132"/>
       <c r="Q61" s="89"/>
       <c r="R61" s="22"/>
       <c r="S61" s="23"/>
@@ -5150,18 +5123,16 @@
         <v>5.8</v>
       </c>
       <c r="L62" s="131" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M62" s="129">
         <v>10.8</v>
       </c>
       <c r="N62" s="129" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O62" s="129"/>
-      <c r="P62" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P62" s="132"/>
       <c r="Q62" s="89"/>
       <c r="R62" s="22"/>
       <c r="S62" s="23"/>
@@ -5207,18 +5178,16 @@
         <v>0.5</v>
       </c>
       <c r="L63" s="131" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M63" s="129">
         <v>8.6</v>
       </c>
       <c r="N63" s="129" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O63" s="129"/>
-      <c r="P63" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P63" s="132"/>
       <c r="Q63" s="89"/>
       <c r="R63" s="22"/>
       <c r="S63" s="23"/>
@@ -5264,18 +5233,16 @@
         <v>13.2</v>
       </c>
       <c r="L64" s="131" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M64" s="129">
         <v>24.8</v>
       </c>
       <c r="N64" s="129" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O64" s="129"/>
-      <c r="P64" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P64" s="132"/>
       <c r="Q64" s="89"/>
       <c r="R64" s="22"/>
       <c r="S64" s="23"/>
@@ -5321,7 +5288,7 @@
         <v>5.7</v>
       </c>
       <c r="L65" s="145" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M65" s="82">
         <v>83</v>
@@ -5356,7 +5323,7 @@
         <v>65</v>
       </c>
       <c r="D66" s="126" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E66" s="127">
         <v>0.85069444444444442</v>
@@ -5380,7 +5347,7 @@
         <v>18.2</v>
       </c>
       <c r="L66" s="131" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M66" s="129">
         <v>57.1</v>
@@ -5389,9 +5356,7 @@
         <v>18</v>
       </c>
       <c r="O66" s="129"/>
-      <c r="P66" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P66" s="132"/>
       <c r="Q66" s="89"/>
       <c r="R66" s="22"/>
       <c r="S66" s="23"/>
@@ -5437,18 +5402,16 @@
         <v>2.6</v>
       </c>
       <c r="L67" s="131" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M67" s="129">
         <v>23.4</v>
       </c>
       <c r="N67" s="129" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O67" s="129"/>
-      <c r="P67" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P67" s="132"/>
       <c r="Q67" s="89"/>
       <c r="R67" s="22"/>
       <c r="S67" s="23"/>
@@ -5470,7 +5433,7 @@
         <v>67</v>
       </c>
       <c r="D68" s="126" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E68" s="127">
         <v>0.9291666666666667</v>
@@ -5494,7 +5457,7 @@
         <v>0</v>
       </c>
       <c r="L68" s="131" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M68" s="129">
         <v>6.2</v>
@@ -5503,9 +5466,7 @@
         <v>18</v>
       </c>
       <c r="O68" s="129"/>
-      <c r="P68" s="132" t="s">
-        <v>30</v>
-      </c>
+      <c r="P68" s="132"/>
       <c r="Q68" s="89"/>
       <c r="R68" s="22"/>
       <c r="S68" s="23"/>
@@ -5527,7 +5488,7 @@
         <v>68</v>
       </c>
       <c r="D69" s="150" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E69" s="80">
         <v>0.88749999999999996</v>
@@ -5551,7 +5512,7 @@
         <v>0.4</v>
       </c>
       <c r="L69" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M69" s="96">
         <v>30.7</v>
@@ -5610,13 +5571,13 @@
         <v>2.4</v>
       </c>
       <c r="L70" s="111" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M70" s="108" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="N70" s="108" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O70" s="112" t="s">
         <v>19</v>
@@ -5669,13 +5630,13 @@
         <v>0.6</v>
       </c>
       <c r="L71" s="97" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M71" s="96" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="N71" s="87" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O71" s="100" t="s">
         <v>19</v>
@@ -5728,7 +5689,7 @@
         <v>3.2</v>
       </c>
       <c r="L72" s="165" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M72" s="166">
         <v>100</v>
@@ -5743,7 +5704,7 @@
         <v>400</v>
       </c>
       <c r="Q72" s="169" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R72" s="22"/>
       <c r="S72" s="22"/>
@@ -5811,7 +5772,7 @@
         <v>1.3</v>
       </c>
       <c r="L73" s="111" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M73" s="108">
         <v>69</v>
@@ -5820,9 +5781,7 @@
         <v>18</v>
       </c>
       <c r="O73" s="108"/>
-      <c r="P73" s="155" t="s">
-        <v>52</v>
-      </c>
+      <c r="P73" s="155"/>
       <c r="Q73" s="89"/>
       <c r="R73" s="22"/>
       <c r="S73" s="23"/>
@@ -5868,7 +5827,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="L74" s="97" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M74" s="96">
         <v>69</v>
@@ -5877,9 +5836,7 @@
         <v>18</v>
       </c>
       <c r="O74" s="95"/>
-      <c r="P74" s="99" t="s">
-        <v>52</v>
-      </c>
+      <c r="P74" s="99"/>
       <c r="Q74" s="89"/>
       <c r="R74" s="22"/>
       <c r="S74" s="23"/>
@@ -5925,7 +5882,7 @@
         <v>1.2</v>
       </c>
       <c r="L75" s="97" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M75" s="96">
         <v>69</v>
@@ -5982,7 +5939,7 @@
         <v>1.6</v>
       </c>
       <c r="L76" s="175" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M76" s="129">
         <v>10.5</v>
@@ -5991,9 +5948,7 @@
         <v>18</v>
       </c>
       <c r="O76" s="129"/>
-      <c r="P76" s="177" t="s">
-        <v>30</v>
-      </c>
+      <c r="P76" s="177"/>
       <c r="Q76" s="89"/>
       <c r="R76" s="22"/>
       <c r="S76" s="23"/>
@@ -6039,7 +5994,7 @@
         <v>1.01</v>
       </c>
       <c r="L77" s="111" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M77" s="108">
         <v>16</v>
@@ -6048,9 +6003,7 @@
         <v>18</v>
       </c>
       <c r="O77" s="108"/>
-      <c r="P77" s="122" t="s">
-        <v>52</v>
-      </c>
+      <c r="P77" s="122"/>
       <c r="Q77" s="89"/>
       <c r="R77" s="22"/>
       <c r="S77" s="23"/>
@@ -6096,7 +6049,7 @@
         <v>1.2</v>
       </c>
       <c r="L78" s="97" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M78" s="96">
         <v>16</v>
@@ -6155,7 +6108,7 @@
         <v>1.3</v>
       </c>
       <c r="L79" s="179" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M79" s="129">
         <v>83</v>
@@ -6164,9 +6117,7 @@
         <v>18</v>
       </c>
       <c r="O79" s="129"/>
-      <c r="P79" s="180" t="s">
-        <v>30</v>
-      </c>
+      <c r="P79" s="180"/>
       <c r="Q79" s="89"/>
       <c r="R79" s="22"/>
       <c r="S79" s="23"/>
@@ -6212,7 +6163,7 @@
         <v>3.2</v>
       </c>
       <c r="L80" s="182" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M80" s="152">
         <v>53</v>
@@ -6221,9 +6172,7 @@
         <v>18</v>
       </c>
       <c r="O80" s="82"/>
-      <c r="P80" s="183" t="s">
-        <v>52</v>
-      </c>
+      <c r="P80" s="183"/>
       <c r="Q80" s="184"/>
       <c r="R80" s="22"/>
       <c r="S80" s="23"/>
@@ -6269,7 +6218,7 @@
         <v>1.4</v>
       </c>
       <c r="L81" s="97" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M81" s="96">
         <v>97.1</v>
@@ -6278,9 +6227,7 @@
         <v>18</v>
       </c>
       <c r="O81" s="95"/>
-      <c r="P81" s="99" t="s">
-        <v>52</v>
-      </c>
+      <c r="P81" s="99"/>
       <c r="Q81" s="89"/>
       <c r="R81" s="22"/>
       <c r="S81" s="23"/>
@@ -6326,7 +6273,7 @@
         <v>2.7</v>
       </c>
       <c r="L82" s="97" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M82" s="96">
         <v>97.1</v>
@@ -6335,9 +6282,7 @@
         <v>18</v>
       </c>
       <c r="O82" s="95"/>
-      <c r="P82" s="99" t="s">
-        <v>52</v>
-      </c>
+      <c r="P82" s="99"/>
       <c r="Q82" s="89"/>
       <c r="R82" s="22"/>
       <c r="S82" s="23"/>
@@ -6383,13 +6328,13 @@
         <v>2.5</v>
       </c>
       <c r="L83" s="97" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M83" s="96" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="N83" s="95" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="O83" s="100" t="s">
         <v>21</v>
@@ -6440,20 +6385,18 @@
         <v>3.7</v>
       </c>
       <c r="L84" s="111" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M84" s="109" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="N84" s="108" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="O84" s="186" t="s">
         <v>21</v>
       </c>
-      <c r="P84" s="122" t="s">
-        <v>52</v>
-      </c>
+      <c r="P84" s="122"/>
       <c r="Q84" s="89"/>
       <c r="R84" s="22"/>
       <c r="S84" s="23"/>
@@ -6499,13 +6442,13 @@
         <v>0</v>
       </c>
       <c r="L85" s="188" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M85" s="84" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="N85" s="87" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="O85" s="189" t="s">
         <v>19</v>
@@ -6534,7 +6477,7 @@
         <v>85</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E86" s="93">
         <v>0.88541666666666663</v>
@@ -6558,7 +6501,7 @@
         <v>2</v>
       </c>
       <c r="L86" s="97" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M86" s="116">
         <v>5.6</v>
@@ -6593,7 +6536,7 @@
         <v>86</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E87" s="93">
         <v>0.89444444444444449</v>
@@ -6617,7 +6560,7 @@
         <v>0</v>
       </c>
       <c r="L87" s="97" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M87" s="95">
         <v>5.6</v>
@@ -6676,7 +6619,7 @@
         <v>1.5</v>
       </c>
       <c r="L88" s="97" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M88" s="96">
         <v>5.6</v>
@@ -6735,13 +6678,13 @@
         <v>1.3</v>
       </c>
       <c r="L89" s="97" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M89" s="96" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N89" s="95" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O89" s="154" t="s">
         <v>19</v>
@@ -6761,7 +6704,7 @@
     </row>
     <row r="90" spans="1:25" ht="16.5" thickTop="1" thickBot="1">
       <c r="A90" s="194" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B90" s="77">
         <v>1</v>
@@ -6794,7 +6737,7 @@
         <v>1.9</v>
       </c>
       <c r="L90" s="182" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M90" s="152">
         <v>100</v>
@@ -6853,7 +6796,7 @@
         <v>4.2</v>
       </c>
       <c r="L91" s="97" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M91" s="96">
         <v>100</v>
@@ -6912,7 +6855,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="L92" s="188" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M92" s="87">
         <v>100</v>
@@ -6921,9 +6864,7 @@
         <v>18</v>
       </c>
       <c r="O92" s="87"/>
-      <c r="P92" s="190" t="s">
-        <v>52</v>
-      </c>
+      <c r="P92" s="190"/>
       <c r="Q92" s="89"/>
       <c r="R92" s="22"/>
       <c r="S92" s="23"/>

</xml_diff>